<commit_message>
att analise de eventos
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos para cada Cenário.xlsx
+++ b/17. Análise de Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalve\Documents\ControlaPet\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368862C4-8FCD-4691-AE85-4B22EA0D8FE7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002374F3-9AE8-47DF-AA9B-70941A307EFD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
   <si>
     <t>Externo</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>X(45)</t>
+  </si>
+  <si>
+    <t>Cliente não autoriza operar animal</t>
+  </si>
+  <si>
+    <t>X(37)</t>
   </si>
 </sst>
 </file>
@@ -552,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -610,84 +616,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -970,12 +979,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1215" activePane="bottomLeft"/>
+      <pane ySplit="1215" topLeftCell="A25" activePane="bottomLeft"/>
       <selection activeCell="D2" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,19 +998,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42" t="s">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42" t="s">
+      <c r="F1" s="36"/>
+      <c r="G1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1035,10 +1044,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="38" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="4">
@@ -1057,8 +1066,8 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="4">
         <v>2</v>
       </c>
@@ -1075,8 +1084,8 @@
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="4">
         <v>3</v>
       </c>
@@ -1093,8 +1102,8 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="4">
         <v>4</v>
       </c>
@@ -1111,8 +1120,8 @@
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="4">
         <v>5</v>
       </c>
@@ -1129,8 +1138,8 @@
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="24">
         <v>6</v>
       </c>
@@ -1147,8 +1156,8 @@
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="40" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="4">
@@ -1167,8 +1176,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4">
         <v>8</v>
       </c>
@@ -1185,8 +1194,8 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4">
         <v>9</v>
       </c>
@@ -1203,8 +1212,8 @@
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="24">
         <v>10</v>
       </c>
@@ -1221,10 +1230,10 @@
       <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="43" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="4">
@@ -1243,8 +1252,8 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="4">
         <v>12</v>
       </c>
@@ -1261,8 +1270,8 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="24">
         <v>13</v>
       </c>
@@ -1279,8 +1288,8 @@
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="27" t="s">
+      <c r="A16" s="42"/>
+      <c r="B16" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="4">
@@ -1299,8 +1308,8 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="24">
         <v>15</v>
       </c>
@@ -1317,10 +1326,10 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="4">
@@ -1339,8 +1348,8 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="4">
         <v>17</v>
       </c>
@@ -1357,8 +1366,8 @@
       <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="33"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="4">
         <v>18</v>
       </c>
@@ -1375,8 +1384,8 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="4">
         <v>19</v>
       </c>
@@ -1393,8 +1402,8 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="4">
         <v>20</v>
       </c>
@@ -1411,8 +1420,8 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="4">
         <v>21</v>
       </c>
@@ -1429,8 +1438,8 @@
       <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="24">
         <v>22</v>
       </c>
@@ -1447,8 +1456,8 @@
       <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="32" t="s">
+      <c r="A25" s="47"/>
+      <c r="B25" s="40" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="4">
@@ -1467,8 +1476,8 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="4">
         <v>24</v>
       </c>
@@ -1485,8 +1494,8 @@
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="33"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="4">
         <v>25</v>
       </c>
@@ -1503,8 +1512,8 @@
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="33"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="4">
         <v>26</v>
       </c>
@@ -1521,8 +1530,8 @@
       <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="33"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="4">
         <v>27</v>
       </c>
@@ -1539,8 +1548,8 @@
       <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39"/>
-      <c r="B30" s="34"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="24">
         <v>28</v>
       </c>
@@ -1557,10 +1566,10 @@
       <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="44" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="4">
@@ -1579,8 +1588,8 @@
       <c r="J31" s="8"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="4">
         <v>30</v>
       </c>
@@ -1597,8 +1606,8 @@
       <c r="J32" s="12"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="4">
         <v>31</v>
       </c>
@@ -1615,8 +1624,8 @@
       <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="44"/>
       <c r="C34" s="4">
         <v>32</v>
       </c>
@@ -1633,8 +1642,8 @@
       <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="4">
         <v>33</v>
       </c>
@@ -1651,8 +1660,8 @@
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="44"/>
       <c r="C36" s="4">
         <v>34</v>
       </c>
@@ -1669,8 +1678,8 @@
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="44"/>
       <c r="C37" s="4">
         <v>35</v>
       </c>
@@ -1687,8 +1696,8 @@
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="44"/>
       <c r="C38" s="4">
         <v>36</v>
       </c>
@@ -1705,8 +1714,8 @@
       <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="45"/>
       <c r="C39" s="24">
         <v>37</v>
       </c>
@@ -1723,8 +1732,8 @@
       <c r="J39" s="19"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="28" t="s">
+      <c r="A40" s="49"/>
+      <c r="B40" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="4">
@@ -1743,8 +1752,8 @@
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="28"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="44"/>
       <c r="C41" s="4">
         <v>39</v>
       </c>
@@ -1761,8 +1770,8 @@
       <c r="J41" s="12"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="44"/>
       <c r="C42" s="4">
         <v>40</v>
       </c>
@@ -1779,8 +1788,8 @@
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="28"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="44"/>
       <c r="C43" s="4">
         <v>41</v>
       </c>
@@ -1797,8 +1806,8 @@
       <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="44"/>
       <c r="C44" s="4">
         <v>42</v>
       </c>
@@ -1814,121 +1823,139 @@
       <c r="I44" s="11"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="26"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="24">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="49"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="53">
         <v>43</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="13"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="15"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="50"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="24">
+        <v>44</v>
+      </c>
+      <c r="D46" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E46" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="19"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
+      <c r="F46" s="17"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="19"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B47" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="4">
-        <v>44</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="46"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
-      <c r="B47" s="33"/>
       <c r="C47" s="4">
         <v>45</v>
       </c>
-      <c r="D47" s="47" t="s">
+      <c r="D47" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" s="25"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="51"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="4">
+        <v>46</v>
+      </c>
+      <c r="D48" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="11" t="s">
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="24">
-        <v>46</v>
-      </c>
-      <c r="D48" s="23" t="s">
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="12"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="51"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="4">
+        <v>47</v>
+      </c>
+      <c r="D49" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="18" t="s">
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="31"/>
-      <c r="B49" s="48" t="s">
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="19"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="52"/>
+      <c r="B50" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="48">
-        <v>47</v>
-      </c>
-      <c r="D49" s="49" t="s">
+      <c r="C50" s="4">
+        <v>48</v>
+      </c>
+      <c r="D50" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="50" t="s">
+      <c r="E50" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="F49" s="50"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="52"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A31:A46"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A30"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B25:B30"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A30"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="A31:A45"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
att analise de eventos 0405
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos para cada Cenário.xlsx
+++ b/17. Análise de Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalve\Documents\ControlaPet\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002374F3-9AE8-47DF-AA9B-70941A307EFD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC86B60-0483-4C8F-A935-A0AA4B2F81C5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>Externo</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>X(37)</t>
+  </si>
+  <si>
+    <t>Cobrar pagamento não efetuado</t>
+  </si>
+  <si>
+    <t>Cadastro não autorizado</t>
   </si>
 </sst>
 </file>
@@ -639,6 +645,54 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,54 +704,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,12 +985,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1215" topLeftCell="A25" activePane="bottomLeft"/>
+      <pane ySplit="1215" activePane="bottomLeft"/>
       <selection activeCell="D2" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,19 +1004,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36" t="s">
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1044,10 +1050,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="42" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="4">
@@ -1066,9 +1072,9 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="4">
+      <c r="A4" s="53"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="34">
         <v>2</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -1084,9 +1090,9 @@
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="4">
+      <c r="A5" s="53"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="34">
         <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1102,9 +1108,9 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="4">
+      <c r="A6" s="53"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="34">
         <v>4</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -1120,9 +1126,9 @@
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="4">
+      <c r="A7" s="53"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="34">
         <v>5</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -1138,8 +1144,8 @@
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="39"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="24">
         <v>6</v>
       </c>
@@ -1156,8 +1162,8 @@
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="53"/>
+      <c r="B9" s="41" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="4">
@@ -1176,9 +1182,9 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="4">
+      <c r="A10" s="53"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="34">
         <v>8</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -1194,203 +1200,199 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="4">
+      <c r="A11" s="53"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="34">
         <v>9</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="53"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="53"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="34">
+        <v>11</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="24">
-        <v>10</v>
-      </c>
-      <c r="D12" s="16" t="s">
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="53"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="24">
+        <v>12</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B15" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4">
-        <v>11</v>
-      </c>
-      <c r="D13" s="20" t="s">
+      <c r="C15" s="4">
+        <v>13</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="4">
-        <v>12</v>
-      </c>
-      <c r="D14" s="21" t="s">
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="45"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="34">
+        <v>14</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="24">
-        <v>13</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4">
-        <v>14</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="24">
         <v>15</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>69</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E17" s="17"/>
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="H17" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="I17" s="18"/>
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>12</v>
+      <c r="A18" s="45"/>
+      <c r="B18" s="46" t="s">
+        <v>20</v>
       </c>
       <c r="C18" s="4">
         <v>16</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="45"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="4">
+      <c r="C19" s="24">
         <v>17</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="12"/>
+      <c r="D19" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>12</v>
+      </c>
       <c r="C20" s="4">
         <v>18</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="12"/>
+      <c r="D20" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="38"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="4">
         <v>19</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>70</v>
@@ -1402,13 +1404,13 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="4">
+      <c r="A22" s="48"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="34">
         <v>20</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>70</v>
@@ -1420,13 +1422,13 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="4">
+      <c r="A23" s="48"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="34">
         <v>21</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>70</v>
@@ -1437,91 +1439,91 @@
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="24">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="48"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="34">
         <v>22</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="48"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="34">
+        <v>23</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="48"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="24">
+        <v>24</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E26" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-    </row>
-    <row r="25" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="40" t="s">
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="48"/>
+      <c r="B27" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="4">
-        <v>23</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="4">
-        <v>24</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="38"/>
       <c r="C27" s="4">
         <v>25</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>52</v>
+      <c r="D27" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="12"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="4">
+      <c r="A28" s="48"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="34">
         <v>26</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="11"/>
@@ -1530,16 +1532,16 @@
       <c r="J28" s="12"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="4">
+      <c r="A29" s="48"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="34">
         <v>27</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="11"/>
@@ -1547,162 +1549,162 @@
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="24">
+      <c r="B30" s="42"/>
+      <c r="C30" s="4">
         <v>28</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="48"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="34">
+        <v>29</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="24">
+        <v>30</v>
+      </c>
+      <c r="D32" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E32" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="19"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="19"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B33" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="4">
-        <v>29</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="4">
-        <v>30</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="44"/>
       <c r="C33" s="4">
         <v>31</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="11" t="s">
+      <c r="D33" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="35"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="34">
+        <v>32</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="15"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="4">
-        <v>32</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="4">
+      <c r="A35" s="35"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="34">
         <v>33</v>
       </c>
       <c r="D35" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="34">
+        <v>34</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="34">
+        <v>35</v>
+      </c>
+      <c r="D37" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="4">
-        <v>34</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="4">
-        <v>35</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F37" s="6"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="4">
+      <c r="A38" s="35"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="34">
         <v>36</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="6" t="s">
@@ -1713,91 +1715,91 @@
       <c r="I38" s="7"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="49"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="24">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="34">
         <v>37</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="35"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="34">
+        <v>38</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="35"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="24">
+        <v>39</v>
+      </c>
+      <c r="D41" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17" t="s">
+      <c r="E41" s="17"/>
+      <c r="F41" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="44" t="s">
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="19"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="35"/>
+      <c r="B42" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="4">
-        <v>38</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="12"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="4">
-        <v>39</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="44"/>
       <c r="C42" s="4">
         <v>40</v>
       </c>
-      <c r="D42" s="21" t="s">
-        <v>35</v>
+      <c r="D42" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" s="10"/>
+        <v>71</v>
+      </c>
+      <c r="F42" s="6"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
       <c r="I42" s="11"/>
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="4">
+      <c r="A43" s="35"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="34">
         <v>41</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>36</v>
+      <c r="D43" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="11"/>
@@ -1806,16 +1808,16 @@
       <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="4">
+      <c r="A44" s="35"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="34">
         <v>42</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="11"/>
@@ -1824,138 +1826,174 @@
       <c r="J44" s="12"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="53">
+      <c r="A45" s="35"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="4">
         <v>43</v>
       </c>
       <c r="D45" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="12"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="35"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="34">
+        <v>44</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="12"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="35"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="34">
+        <v>45</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E47" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="15"/>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="50"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="24">
-        <v>44</v>
-      </c>
-      <c r="D46" s="23" t="s">
+      <c r="F47" s="13"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="15"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="36"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="24">
+        <v>46</v>
+      </c>
+      <c r="D48" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E48" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="19"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="51" t="s">
+      <c r="F48" s="17"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="19"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B49" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="4">
-        <v>45</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="51"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="4">
-        <v>46</v>
-      </c>
-      <c r="D48" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="12"/>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="51"/>
-      <c r="B49" s="39"/>
       <c r="C49" s="4">
         <v>47</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="25"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="39"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="34">
+        <v>48</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="39"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="24">
+        <v>49</v>
+      </c>
+      <c r="D51" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="18" t="s">
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="19"/>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="52"/>
-      <c r="B50" s="29" t="s">
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="19"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="40"/>
+      <c r="B52" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="4">
-        <v>48</v>
-      </c>
-      <c r="D50" s="30" t="s">
+      <c r="C52" s="4">
+        <v>50</v>
+      </c>
+      <c r="D52" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E52" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="F50" s="31"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="33"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A31:A46"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B40:B46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A30"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B30"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A3:A14"/>
     <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A32"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="A33:A48"/>
+    <mergeCell ref="B33:B41"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Correcao segundo orientacao do professor 1505
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos para cada Cenário.xlsx
+++ b/17. Análise de Eventos para cada Cenário.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalve\Documents\ControlaPet\Artefatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\ControlaPet\Artefatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC86B60-0483-4C8F-A935-A0AA4B2F81C5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A34006-B81B-40C4-95C1-D6C66CC894EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
   <si>
     <t>Externo</t>
   </si>
@@ -162,36 +162,9 @@
     <t>Cliente solicita consulta</t>
   </si>
   <si>
-    <t>Cliente autoriza medicação</t>
-  </si>
-  <si>
-    <t>Cliente autoriza consulta</t>
-  </si>
-  <si>
-    <t>Cliente autoriza alimentar animal</t>
-  </si>
-  <si>
-    <t>Cliente autoriza passear com animal</t>
-  </si>
-  <si>
-    <t>Cliente autoriza banhar animal</t>
-  </si>
-  <si>
     <t>Cliente solicita fechar conta</t>
   </si>
   <si>
-    <t>Cliente não autoriza banhar animal</t>
-  </si>
-  <si>
-    <t>Cliente não autoriza passear com animal</t>
-  </si>
-  <si>
-    <t>Cliente não autoriza alimentar animal</t>
-  </si>
-  <si>
-    <t>Cliente não autoriza consulta</t>
-  </si>
-  <si>
     <t>Veterinária consulta histórico</t>
   </si>
   <si>
@@ -237,9 +210,6 @@
     <t>X(12)</t>
   </si>
   <si>
-    <t>X(16)</t>
-  </si>
-  <si>
     <t>X(29)</t>
   </si>
   <si>
@@ -252,21 +222,9 @@
     <t>Fim do dia: Recepcionista registra comissão de funcionarios</t>
   </si>
   <si>
-    <t>X(17)</t>
-  </si>
-  <si>
     <t>X(18)</t>
   </si>
   <si>
-    <t>X(19)</t>
-  </si>
-  <si>
-    <t>X(21)</t>
-  </si>
-  <si>
-    <t>X(20)</t>
-  </si>
-  <si>
     <t>X(33)</t>
   </si>
   <si>
@@ -295,6 +253,24 @@
   </si>
   <si>
     <t>Cadastro não autorizado</t>
+  </si>
+  <si>
+    <t>Caseiro alimenta animal</t>
+  </si>
+  <si>
+    <t>Caseiro encaminha para banho</t>
+  </si>
+  <si>
+    <t>Caseiro encaminha para consulta</t>
+  </si>
+  <si>
+    <t>Caseiro encaminha para medicamento</t>
+  </si>
+  <si>
+    <t>x(18)</t>
+  </si>
+  <si>
+    <t>Caseiro passeia com animal</t>
   </si>
 </sst>
 </file>
@@ -564,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,9 +666,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,6 +678,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,12 +962,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1215" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1215" topLeftCell="A13" activePane="bottomLeft"/>
       <selection activeCell="D2" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,19 +981,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52" t="s">
+      <c r="F1" s="51"/>
+      <c r="G1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1050,7 +1027,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="52" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="42" t="s">
@@ -1072,7 +1049,7 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="42"/>
       <c r="C4" s="34">
         <v>2</v>
@@ -1081,7 +1058,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
@@ -1090,7 +1067,7 @@
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="42"/>
       <c r="C5" s="34">
         <v>3</v>
@@ -1108,7 +1085,7 @@
       <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="42"/>
       <c r="C6" s="34">
         <v>4</v>
@@ -1117,7 +1094,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="11"/>
@@ -1126,7 +1103,7 @@
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="42"/>
       <c r="C7" s="34">
         <v>5</v>
@@ -1135,7 +1112,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
@@ -1144,7 +1121,7 @@
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="43"/>
       <c r="C8" s="24">
         <v>6</v>
@@ -1155,14 +1132,14 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="18" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="41" t="s">
         <v>20</v>
       </c>
@@ -1173,7 +1150,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
@@ -1182,7 +1159,7 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="42"/>
       <c r="C10" s="34">
         <v>8</v>
@@ -1191,7 +1168,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
@@ -1200,13 +1177,13 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="42"/>
       <c r="C11" s="34">
         <v>9</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1216,13 +1193,13 @@
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="42"/>
       <c r="C12" s="4">
         <v>10</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1232,7 +1209,7 @@
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="42"/>
       <c r="C13" s="34">
         <v>11</v>
@@ -1245,12 +1222,12 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="43"/>
       <c r="C14" s="24">
         <v>12</v>
@@ -1259,7 +1236,7 @@
         <v>24</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="18"/>
@@ -1281,7 +1258,7 @@
         <v>26</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
@@ -1299,7 +1276,7 @@
         <v>27</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
@@ -1314,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -1337,7 +1314,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
@@ -1355,7 +1332,7 @@
         <v>29</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
@@ -1392,13 +1369,13 @@
         <v>19</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
+      <c r="G21" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
@@ -1410,13 +1387,13 @@
         <v>20</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="12"/>
@@ -1428,13 +1405,13 @@
         <v>21</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
@@ -1446,13 +1423,13 @@
         <v>22</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="12"/>
@@ -1464,13 +1441,13 @@
         <v>23</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
@@ -1482,10 +1459,10 @@
         <v>24</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -1493,133 +1470,133 @@
       <c r="I26" s="18"/>
       <c r="J26" s="19"/>
     </row>
-    <row r="27" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="48"/>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="29">
         <v>25</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="34">
-        <v>26</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>75</v>
+      <c r="E27" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="33"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4">
+        <v>31</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
-      <c r="B29" s="42"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="34">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="4">
-        <v>28</v>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="35"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="34">
+        <v>33</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="42"/>
+        <v>46</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="35"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="34">
-        <v>29</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="49"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="24">
-        <v>30</v>
-      </c>
-      <c r="D32" s="23" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="35"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="34">
+        <v>35</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="34">
         <v>36</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="4">
-        <v>31</v>
-      </c>
       <c r="D33" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -1629,354 +1606,264 @@
       <c r="A34" s="35"/>
       <c r="B34" s="37"/>
       <c r="C34" s="34">
-        <v>32</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="12"/>
+      <c r="F34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
       <c r="B35" s="37"/>
       <c r="C35" s="34">
-        <v>33</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="15"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="34">
-        <v>34</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10" t="s">
+      <c r="B36" s="38"/>
+      <c r="C36" s="24">
+        <v>39</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="12"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="19"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="34">
-        <v>35</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>72</v>
+      <c r="B37" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="4">
+        <v>40</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="F37" s="6"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="8"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" s="37"/>
       <c r="C38" s="34">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" s="37"/>
       <c r="C39" s="34">
-        <v>37</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" s="37"/>
-      <c r="C40" s="34">
-        <v>38</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="4">
+        <v>43</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="24">
-        <v>39</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="34">
+        <v>44</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="12"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
-      <c r="B42" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="4">
+      <c r="B42" s="37"/>
+      <c r="C42" s="34">
+        <v>45</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="36"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="24">
+        <v>46</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="19"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="4">
+        <v>47</v>
+      </c>
+      <c r="D44" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="12"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="34">
+      <c r="E44" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="39"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="34">
+        <v>48</v>
+      </c>
+      <c r="D45" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="12"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="34">
-        <v>42</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="12"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="4">
-        <v>43</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="E45" s="10"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="11"/>
+      <c r="G45" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="34">
-        <v>44</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="12"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="34">
-        <v>45</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="15"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="36"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="24">
-        <v>46</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="4">
-        <v>47</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F49" s="25"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="27"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="39"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="34">
-        <v>48</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="12"/>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="39"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="24">
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="39"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="24">
         <v>49</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="D46" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="19"/>
-    </row>
-    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="40"/>
-      <c r="B52" s="29" t="s">
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="19"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="40"/>
+      <c r="B47" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C47" s="4">
         <v>50</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D47" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" s="31"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="33"/>
+      <c r="E47" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" s="31"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
@@ -1986,14 +1873,13 @@
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A32"/>
+    <mergeCell ref="A20:A27"/>
     <mergeCell ref="B20:B26"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="A33:A48"/>
-    <mergeCell ref="B33:B41"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A28:A43"/>
+    <mergeCell ref="B28:B36"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>